<commit_message>
Archivos nuevos,no se cuales
</commit_message>
<xml_diff>
--- a/documentacion/copy/df_sucio.xlsx
+++ b/documentacion/copy/df_sucio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D122"/>
+  <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,10 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>Nombre</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
@@ -454,15 +449,12 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Daniel Esteban Romero Romero</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
-        <is>
-          <t>Daniel Esteban Romero Romero</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
         <is>
           <t>https://es-la.facebook.com/people/Daniel-Esteban-Romero/pfbid08AtEbiPfUSHBJTgQ24VeSteyyXhG4dw5Fbs1W3B9cUheM7WRBxLanfuKgZLEprAal/</t>
         </is>
@@ -472,15 +464,12 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
-        <v>2</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Jersson Steven Castillo Romero</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
-        <is>
-          <t>Jersson Steven Castillo Romero</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
         <is>
           <t>https://oga.bogota.unal.edu.co/certificados/20171/p12.pdf</t>
         </is>
@@ -490,15 +479,12 @@
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
-        <v>3</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Wilmar Jair Gomez Rios</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
-        <is>
-          <t>Wilmar Jair Gomez Rios</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
         <is>
           <t>https://www.uniagraria.edu.co/wp-content/uploads/2021/03/formato-Hoja-de-vida-UNIAGRARIA-Wilmar-G%C3%B3mez.pdf</t>
         </is>
@@ -508,15 +494,12 @@
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
-        <v>4</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Jonathan Francisco Ballesteros Cubillos</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
-        <is>
-          <t>Jonathan Francisco Ballesteros Cubillos</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
         <is>
           <t>https://co.pinterest.com/joncito9311/</t>
         </is>
@@ -526,15 +509,12 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
-        <v>5</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Guillermo Sanchez Herrera</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
-        <is>
-          <t>Guillermo Sanchez Herrera</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
         <is>
           <t>https://scholar.google.com/citations?user=0VMTl4IAAAAJ&amp;hl=es</t>
         </is>
@@ -544,15 +524,12 @@
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
-        <v>6</v>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Cristian Camilo Ortiz Yara</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
-        <is>
-          <t>Cristian Camilo Ortiz Yara</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
         <is>
           <t>https://www.youtube.com/channel/UCkzQeSBaLSecTl5r2n-m1uw</t>
         </is>
@@ -562,15 +539,12 @@
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
-        <v>7</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Luis Miguel Martinez Largo</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
-        <is>
-          <t>Luis Miguel Martinez Largo</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>https://www.youtube.com/channel/UCQBUllbV2HylTRnZgHqGMBQ</t>
         </is>
@@ -580,15 +554,12 @@
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
-        <v>8</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Jhonatan Andres Quintero Tolosa</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
-        <is>
-          <t>Jhonatan Andres Quintero Tolosa</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
         <is>
           <t>https://www.facebook.com/jhonatan.tolosa/</t>
         </is>
@@ -598,15 +569,12 @@
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
-        <v>9</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Angélica María Suárez Sarmiento</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
-        <is>
-          <t>Angélica María Suárez Sarmiento</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
         <is>
           <t>https://es-la.facebook.com/Angelicamaria.suarezsarmiento/</t>
         </is>
@@ -616,15 +584,12 @@
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
-        <v>10</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Luis Felipe Rico Cortes</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
-        <is>
-          <t>Luis Felipe Rico Cortes</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
         <is>
           <t>https://www.uni-due.de/empi/cfd/en/felipe.php</t>
         </is>
@@ -634,15 +599,12 @@
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
-        <v>11</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>José Alejandro Zúñiga Claro</t>
+        </is>
       </c>
       <c r="C12" t="inlineStr">
-        <is>
-          <t>José Alejandro Zúñiga Claro</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
         <is>
           <t>https://www.youtube.com/user/alejandrozone?app=desktop</t>
         </is>
@@ -652,15 +614,12 @@
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="n">
-        <v>12</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Jaime Alejandro Novoa Usaquen</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
-        <is>
-          <t>Jaime Alejandro Novoa Usaquen</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
         <is>
           <t>https://www.habitatbogota.gov.co/transparencia/normativa/notificaciones/jaime-alejandro-novoa-usaquen</t>
         </is>
@@ -670,15 +629,12 @@
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="n">
-        <v>13</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>John Alexander Quiroga Olaya</t>
+        </is>
       </c>
       <c r="C14" t="inlineStr">
-        <is>
-          <t>John Alexander Quiroga Olaya</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
         <is>
           <t>https://sci.org.co/john-alexander-quiroga-olaya/</t>
         </is>
@@ -688,15 +644,12 @@
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
-        <v>14</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Julian David Madrid Leal</t>
+        </is>
       </c>
       <c r="C15" t="inlineStr">
-        <is>
-          <t>Julian David Madrid Leal</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
         <is>
           <t>https://construyored.com/profesionales/9633-julian-david-madrid-leal</t>
         </is>
@@ -706,15 +659,12 @@
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="n">
-        <v>15</v>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Louis Edwards Caceres Martinez</t>
+        </is>
       </c>
       <c r="C16" t="inlineStr">
-        <is>
-          <t>Louis Edwards Caceres Martinez</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
         <is>
           <t>https://scholar.google.com/citations?user=WPk9UTAAAAAJ&amp;hl=es</t>
         </is>
@@ -724,15 +674,12 @@
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="n">
-        <v>16</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Jaime Quintero Sarmiento</t>
+        </is>
       </c>
       <c r="C17" t="inlineStr">
-        <is>
-          <t>Jaime Quintero Sarmiento</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
         <is>
           <t>https://es-la.facebook.com/jaimeqs1/</t>
         </is>
@@ -742,15 +689,12 @@
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="n">
-        <v>17</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Ricardo Antonio Diaz Herrera</t>
+        </is>
       </c>
       <c r="C18" t="inlineStr">
-        <is>
-          <t>Ricardo Antonio Diaz Herrera</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
         <is>
           <t>https://es-la.facebook.com/ricardo.a.herrera.73/</t>
         </is>
@@ -760,15 +704,12 @@
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="n">
-        <v>18</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Irving Attara Martinez</t>
+        </is>
       </c>
       <c r="C19" t="inlineStr">
-        <is>
-          <t>Irving Attara Martinez</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
         <is>
           <t>https://www.bazzarbog.com/shop/irving-attara-martinez</t>
         </is>
@@ -778,15 +719,12 @@
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="n">
-        <v>19</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Maximiliano Vargas Cortes</t>
+        </is>
       </c>
       <c r="C20" t="inlineStr">
-        <is>
-          <t>Maximiliano Vargas Cortes</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
         <is>
           <t>https://www.facebook.com/maximiliano.v.cortes.1/?locale=es_ES</t>
         </is>
@@ -796,15 +734,12 @@
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="n">
-        <v>20</v>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Juan David Lozada Trujillo</t>
+        </is>
       </c>
       <c r="C21" t="inlineStr">
-        <is>
-          <t>Juan David Lozada Trujillo</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
         <is>
           <t>https://es-la.facebook.com/Pandaman.Lozada/</t>
         </is>
@@ -814,15 +749,12 @@
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="n">
-        <v>21</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Carlos Eduardo Hernandez Carvajal</t>
+        </is>
       </c>
       <c r="C22" t="inlineStr">
-        <is>
-          <t>Carlos Eduardo Hernandez Carvajal</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
         <is>
           <t>https://www.instagram.com/carlos.hernandez.carvajal/?hl=es-la</t>
         </is>
@@ -832,15 +764,12 @@
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" t="n">
-        <v>22</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>David Andres Baquero Ramirez</t>
+        </is>
       </c>
       <c r="C23" t="inlineStr">
-        <is>
-          <t>David Andres Baquero Ramirez</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
         <is>
           <t>https://repositorio.unal.edu.co/handle/unal/21/browse?type=author&amp;value=Baquero+Ramirez%2C+David+Andres</t>
         </is>
@@ -850,15 +779,12 @@
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" t="n">
-        <v>23</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Victor Daniel Alfonso Peña</t>
+        </is>
       </c>
       <c r="C24" t="inlineStr">
-        <is>
-          <t>Victor Daniel Alfonso Peña</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
         <is>
           <t>http://www.datajuridica.com/ALFONSO_PE%C3%91A.htm</t>
         </is>
@@ -868,15 +794,12 @@
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" t="n">
-        <v>24</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Andres David Gonzalez Ortiz</t>
+        </is>
       </c>
       <c r="C25" t="inlineStr">
-        <is>
-          <t>Andres David Gonzalez Ortiz</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
         <is>
           <t>https://m.facebook.com/andresdavid.gonzalezortiz/</t>
         </is>
@@ -886,15 +809,12 @@
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" t="n">
-        <v>25</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Camilo Andres Pinzon Ruiz</t>
+        </is>
       </c>
       <c r="C26" t="inlineStr">
-        <is>
-          <t>Camilo Andres Pinzon Ruiz</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
         <is>
           <t>https://www.facebook.com/camiloar1/?locale=es_LA</t>
         </is>
@@ -904,15 +824,12 @@
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" t="n">
-        <v>26</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Elma Bibiam Naranjo Estepa</t>
+        </is>
       </c>
       <c r="C27" t="inlineStr">
-        <is>
-          <t>Elma Bibiam Naranjo Estepa</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
         <is>
           <t>https://repositorio.unal.edu.co/browse?type=author&amp;value=Naranjo%20Estepa,%20Elma%20Bibiam</t>
         </is>
@@ -922,15 +839,12 @@
       <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B28" t="n">
-        <v>27</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Gabriel Alejandro Hidalgo Lagos</t>
+        </is>
       </c>
       <c r="C28" t="inlineStr">
-        <is>
-          <t>Gabriel Alejandro Hidalgo Lagos</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
         <is>
           <t>https://www.tusclases.co/profesores/gabriel-alejandro-hidalgo-lagos.htm</t>
         </is>
@@ -940,15 +854,12 @@
       <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B29" t="n">
-        <v>28</v>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Andrés Felipe Cantor Albarracín</t>
+        </is>
       </c>
       <c r="C29" t="inlineStr">
-        <is>
-          <t>Andrés Felipe Cantor Albarracín</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
         <is>
           <t>https://repositorio.unal.edu.co/browse?type=author&amp;value=Cantor%20Albarrac%C3%ADn,%20Andr%C3%A9s%20Felipe</t>
         </is>
@@ -958,15 +869,12 @@
       <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B30" t="n">
-        <v>29</v>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Diana Johanna Cogua Romero</t>
+        </is>
       </c>
       <c r="C30" t="inlineStr">
-        <is>
-          <t>Diana Johanna Cogua Romero</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
         <is>
           <t>https://www.funcionpublica.gov.co/fdci/consultaCiudadana/index?find=FindNext&amp;tipoPersonaId=25&amp;tipoDeclaracionId=&amp;razonSocial=&amp;primerApellido=&amp;primerNombre=&amp;segundoApellido=&amp;segundoNombre=&amp;numeroDocumento=&amp;entidad=&amp;fechaFinalizacionDesde=08%2F11%2F2021&amp;fechaFinalizacionHasta=&amp;sort=numeroFormulario&amp;max=10&amp;offset=227760&amp;order=asc#resultadosBusqueda</t>
         </is>
@@ -976,15 +884,12 @@
       <c r="A31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B31" t="n">
-        <v>30</v>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Camilo Andres Molina Suarez</t>
+        </is>
       </c>
       <c r="C31" t="inlineStr">
-        <is>
-          <t>Camilo Andres Molina Suarez</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
         <is>
           <t>https://hi-in.facebook.com/public/Camilo-Andres-Suarez-Molina/</t>
         </is>
@@ -994,15 +899,12 @@
       <c r="A32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B32" t="n">
-        <v>31</v>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Henry Felipe Velandia Larrotta</t>
+        </is>
       </c>
       <c r="C32" t="inlineStr">
-        <is>
-          <t>Henry Felipe Velandia Larrotta</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
         <is>
           <t>https://losestudiantes.com/universidad-nacional/professors/henry-felipe-velandia-larrota</t>
         </is>
@@ -1012,15 +914,12 @@
       <c r="A33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B33" t="n">
-        <v>32</v>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Sebastian Ernesto Sierra Loaiza</t>
+        </is>
       </c>
       <c r="C33" t="inlineStr">
-        <is>
-          <t>Sebastian Ernesto Sierra Loaiza</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
         <is>
           <t>https://scholar.google.com.co/citations?user=ZK7b4FcAAAAJ&amp;hl=es</t>
         </is>
@@ -1030,15 +929,12 @@
       <c r="A34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B34" t="n">
-        <v>33</v>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Osbaldo Fabián Viasus Salcedo</t>
+        </is>
       </c>
       <c r="C34" t="inlineStr">
-        <is>
-          <t>Osbaldo Fabián Viasus Salcedo</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
         <is>
           <t>https://www.academia.edu/36898239/Osbaldo_Fabi%C3%A1n_Vias%C3%BAs_Salcedo_HOJA_DE_VIDA</t>
         </is>
@@ -1048,15 +944,12 @@
       <c r="A35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B35" t="n">
-        <v>34</v>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Jr Martin Jurado Realpe</t>
+        </is>
       </c>
       <c r="C35" t="inlineStr">
-        <is>
-          <t>Jr Martin Jurado Realpe</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
         <is>
           <t>https://gite.lirmm.fr/juradoreal</t>
         </is>
@@ -1066,15 +959,12 @@
       <c r="A36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B36" t="n">
-        <v>35</v>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Luis Gabriel Tutacha Coral</t>
+        </is>
       </c>
       <c r="C36" t="inlineStr">
-        <is>
-          <t>Luis Gabriel Tutacha Coral</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
         <is>
           <t>https://enfermeria.bogota.unal.edu.co/fileadmin/Portafolio_de_Servicios/Unidad_Administrativa/ORDENES_CONTRACTUALES_DE_PRESTACION_DE_SERVICIOS_EMPRESA_2016_Y_2066_-_ENERO_A_DICIEMBRE_DE__2017.pdf</t>
         </is>
@@ -1084,15 +974,12 @@
       <c r="A37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B37" t="n">
-        <v>36</v>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Anderson Kavir Osorio Delgado</t>
+        </is>
       </c>
       <c r="C37" t="inlineStr">
-        <is>
-          <t>Anderson Kavir Osorio Delgado</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
         <is>
           <t>https://repositorio.unal.edu.co/handle/unal/80482</t>
         </is>
@@ -1102,15 +989,12 @@
       <c r="A38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B38" t="n">
-        <v>37</v>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Viviana Marcela Varon Ramirez</t>
+        </is>
       </c>
       <c r="C38" t="inlineStr">
-        <is>
-          <t>Viviana Marcela Varon Ramirez</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
         <is>
           <t>https://scholar.google.com/citations?user=-spxm8MAAAAJ&amp;hl=es</t>
         </is>
@@ -1120,15 +1004,12 @@
       <c r="A39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B39" t="n">
-        <v>38</v>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Nelson Fabian Lopez Santamaria</t>
+        </is>
       </c>
       <c r="C39" t="inlineStr">
-        <is>
-          <t>Nelson Fabian Lopez Santamaria</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
         <is>
           <t>https://repositorio.unal.edu.co/browse?type=author&amp;value=L%C3%B3pez%20Santamar%C3%ADa,%20Nelson%20Fabi%C3%A1n</t>
         </is>
@@ -1138,15 +1019,12 @@
       <c r="A40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B40" t="n">
-        <v>39</v>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Daniel Enrique Duque Arias</t>
+        </is>
       </c>
       <c r="C40" t="inlineStr">
-        <is>
-          <t>Daniel Enrique Duque Arias</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
         <is>
           <t>https://consorcioqutubminar.com/team/profileDaniel.html</t>
         </is>
@@ -1156,15 +1034,12 @@
       <c r="A41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B41" t="n">
-        <v>40</v>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Camilo Jose Baquero Baquero</t>
+        </is>
       </c>
       <c r="C41" t="inlineStr">
-        <is>
-          <t>Camilo Jose Baquero Baquero</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
         <is>
           <t>https://www.instagram.com/josebaqueroh/?hl=es</t>
         </is>
@@ -1174,15 +1049,12 @@
       <c r="A42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B42" t="n">
-        <v>41</v>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Jhon Edison Arango Oviedo</t>
+        </is>
       </c>
       <c r="C42" t="inlineStr">
-        <is>
-          <t>Jhon Edison Arango Oviedo</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
         <is>
           <t>https://www.instagram.com/balletmetropolitano/?utm_source=ig_embed&amp;ig_rid=3cfb8116-3b71-4e85-bf7c-133732e73c8f&amp;ig_mid=21CCAAD7-7BE6-4C95-A6ED-F34F96F082D4</t>
         </is>
@@ -1192,15 +1064,12 @@
       <c r="A43" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B43" t="n">
-        <v>42</v>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Wilman Yesid Quintero Barbosa</t>
+        </is>
       </c>
       <c r="C43" t="inlineStr">
-        <is>
-          <t>Wilman Yesid Quintero Barbosa</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
         <is>
           <t>https://revista.redipe.org/index.php/1/article/view/2013</t>
         </is>
@@ -1210,15 +1079,12 @@
       <c r="A44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B44" t="n">
-        <v>43</v>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Daniel Alejandro Saenz Ayerbe</t>
+        </is>
       </c>
       <c r="C44" t="inlineStr">
-        <is>
-          <t>Daniel Alejandro Saenz Ayerbe</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
         <is>
           <t>https://es-la.facebook.com/people/Daniel-Alejandro-S%C3%A1enz-Ayerbe/pfbid02XDPzmDDb7HQnTwdbhWTV1EDaEbaXVFrocPPHCcaQw7qf8F2ej32vsry9DNcjRWXVl/</t>
         </is>
@@ -1228,15 +1094,12 @@
       <c r="A45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B45" t="n">
-        <v>44</v>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Fabian Andres Farfan Mahecha</t>
+        </is>
       </c>
       <c r="C45" t="inlineStr">
-        <is>
-          <t>Fabian Andres Farfan Mahecha</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
         <is>
           <t>https://www.youtube.com/channel/UCehp5YabyzOVPdE7WUynN2A/channels?app=desktop&amp;view=56&amp;shelf_id=0</t>
         </is>
@@ -1246,15 +1109,12 @@
       <c r="A46" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B46" t="n">
-        <v>45</v>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Juan David Mongui Rojas</t>
+        </is>
       </c>
       <c r="C46" t="inlineStr">
-        <is>
-          <t>Juan David Mongui Rojas</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
         <is>
           <t>https://www.facebook.com/unal.ing.bog/photos/a.478608325484001/1280013788676780/?type=3</t>
         </is>
@@ -1264,15 +1124,12 @@
       <c r="A47" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B47" t="n">
-        <v>46</v>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Camilo Alberto Duarte Cordon</t>
+        </is>
       </c>
       <c r="C47" t="inlineStr">
-        <is>
-          <t>Camilo Alberto Duarte Cordon</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
         <is>
           <t>https://scholar.google.com/citations?user=d1GtGzgAAAAJ&amp;hl=en</t>
         </is>
@@ -1282,15 +1139,12 @@
       <c r="A48" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B48" t="n">
-        <v>47</v>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Jairo Andrés Neuta Bernal</t>
+        </is>
       </c>
       <c r="C48" t="inlineStr">
-        <is>
-          <t>Jairo Andrés Neuta Bernal</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
         <is>
           <t>https://www.youtube.com/channel/UCobrnUWc2wxydob_LhUuIGQ</t>
         </is>
@@ -1300,15 +1154,12 @@
       <c r="A49" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B49" t="n">
-        <v>48</v>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Miguel Angel Ruiz Moya</t>
+        </is>
       </c>
       <c r="C49" t="inlineStr">
-        <is>
-          <t>Miguel Angel Ruiz Moya</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
         <is>
           <t>https://www.facebook.com/miguelangel.ruizmoya/?locale=es_ES</t>
         </is>
@@ -1318,15 +1169,12 @@
       <c r="A50" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B50" t="n">
-        <v>49</v>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Javier Becerra Garavito</t>
+        </is>
       </c>
       <c r="C50" t="inlineStr">
-        <is>
-          <t>Javier Becerra Garavito</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
         <is>
           <t>https://www.facebook.com/jhoangaravito/?locale=es_LA</t>
         </is>
@@ -1336,15 +1184,12 @@
       <c r="A51" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B51" t="n">
-        <v>50</v>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Santiago Marquez Ortiz</t>
+        </is>
       </c>
       <c r="C51" t="inlineStr">
-        <is>
-          <t>Santiago Marquez Ortiz</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
         <is>
           <t>https://www.facebook.com/santiago.marquezortiz/</t>
         </is>
@@ -1354,15 +1199,12 @@
       <c r="A52" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B52" t="n">
-        <v>51</v>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Edwin Leonardo Bohorquez Buitrago</t>
+        </is>
       </c>
       <c r="C52" t="inlineStr">
-        <is>
-          <t>Edwin Leonardo Bohorquez Buitrago</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
         <is>
           <t>https://torre.ai/elbohorquez?r=T93fZ1sj</t>
         </is>
@@ -1372,15 +1214,12 @@
       <c r="A53" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B53" t="n">
-        <v>52</v>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Jorge Luis Castañeda Lesmes</t>
+        </is>
       </c>
       <c r="C53" t="inlineStr">
-        <is>
-          <t>Jorge Luis Castañeda Lesmes</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
         <is>
           <t>https://colibri.veeduriadistrital.gov.co/sites/default/files/2021-12/Acta_asistencia_05_04052021_uatmayo_bosa%20%282%29.pdf</t>
         </is>
@@ -1390,15 +1229,12 @@
       <c r="A54" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B54" t="n">
-        <v>53</v>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Andres Felipe Ospina Triviño</t>
+        </is>
       </c>
       <c r="C54" t="inlineStr">
-        <is>
-          <t>Andres Felipe Ospina Triviño</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
         <is>
           <t>https://www.researchgate.net/profile/Andres-Felipe-Ospina-Trivino-2</t>
         </is>
@@ -1408,15 +1244,12 @@
       <c r="A55" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B55" t="n">
-        <v>54</v>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Eduar Barajas Higuera</t>
+        </is>
       </c>
       <c r="C55" t="inlineStr">
-        <is>
-          <t>Eduar Barajas Higuera</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
         <is>
           <t>https://www.facebook.com/eduard.higuera/?locale=es_LA</t>
         </is>
@@ -1426,15 +1259,12 @@
       <c r="A56" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B56" t="n">
-        <v>55</v>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Leidy Nathalia Tabares Ordoñez</t>
+        </is>
       </c>
       <c r="C56" t="inlineStr">
-        <is>
-          <t>Leidy Nathalia Tabares Ordoñez</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
         <is>
           <t>https://construyored.com/profesionales/7538-leidy-nathalia-tabares-ordonez</t>
         </is>
@@ -1444,15 +1274,12 @@
       <c r="A57" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B57" t="n">
-        <v>56</v>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Juan David Cepeda Solarte</t>
+        </is>
       </c>
       <c r="C57" t="inlineStr">
-        <is>
-          <t>Juan David Cepeda Solarte</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
         <is>
           <t>https://www.researchgate.net/profile/Juan-David-Cepeda-Solarte</t>
         </is>
@@ -1462,15 +1289,12 @@
       <c r="A58" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B58" t="n">
-        <v>57</v>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>David Felipe Peñuela Beltrán</t>
+        </is>
       </c>
       <c r="C58" t="inlineStr">
-        <is>
-          <t>David Felipe Peñuela Beltrán</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
         <is>
           <t>https://www.facebook.com/davidfpenuelab/</t>
         </is>
@@ -1480,15 +1304,12 @@
       <c r="A59" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B59" t="n">
-        <v>58</v>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Monica Adriana Vaca Umaña</t>
+        </is>
       </c>
       <c r="C59" t="inlineStr">
-        <is>
-          <t>Monica Adriana Vaca Umaña</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
         <is>
           <t>https://repositorio.unal.edu.co/handle/unal/8/browse?type=author&amp;value=Vaca+Uma%C3%B1a%2C+M%C3%B3nica+Adriana</t>
         </is>
@@ -1498,15 +1319,12 @@
       <c r="A60" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B60" t="n">
-        <v>59</v>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Yulitza Stephanie Ángel López</t>
+        </is>
       </c>
       <c r="C60" t="inlineStr">
-        <is>
-          <t>Yulitza Stephanie Ángel López</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
         <is>
           <t>https://independent.academia.edu/YulitzaStephanieangelLopez</t>
         </is>
@@ -1516,15 +1334,12 @@
       <c r="A61" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B61" t="n">
-        <v>60</v>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Luis Carlos Gutierrez Peña</t>
+        </is>
       </c>
       <c r="C61" t="inlineStr">
-        <is>
-          <t>Luis Carlos Gutierrez Peña</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
         <is>
           <t>https://repositoriousco.co/bitstream/123456789/2624/1/EE%200031.pdf</t>
         </is>
@@ -1534,15 +1349,12 @@
       <c r="A62" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B62" t="n">
-        <v>61</v>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Laura Melisa Martinez Olivella</t>
+        </is>
       </c>
       <c r="C62" t="inlineStr">
-        <is>
-          <t>Laura Melisa Martinez Olivella</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
         <is>
           <t>https://swe.org/brasil/laura-melisa-martinez-olivella/</t>
         </is>
@@ -1552,15 +1364,12 @@
       <c r="A63" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B63" t="n">
-        <v>62</v>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Johan Erik Fajardo Cepeda</t>
+        </is>
       </c>
       <c r="C63" t="inlineStr">
-        <is>
-          <t>Johan Erik Fajardo Cepeda</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
         <is>
           <t>https://www.fiscalia.gov.co/colombia/wp-content/uploads/Escrito-de-Tutela-Jhony-Junior-Chadid-Blanco-2023-03.pdf</t>
         </is>
@@ -1570,15 +1379,12 @@
       <c r="A64" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B64" t="n">
-        <v>63</v>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Fabian Leonardo Guerrero Rojas</t>
+        </is>
       </c>
       <c r="C64" t="inlineStr">
-        <is>
-          <t>Fabian Leonardo Guerrero Rojas</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
         <is>
           <t>https://www.youtube.com/channel/UC6YgocTHXN9D1HObjBTiIUA</t>
         </is>
@@ -1588,15 +1394,12 @@
       <c r="A65" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B65" t="n">
-        <v>64</v>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Pablo Andres Cubides Guerrero</t>
+        </is>
       </c>
       <c r="C65" t="inlineStr">
-        <is>
-          <t>Pablo Andres Cubides Guerrero</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
         <is>
           <t>https://repositorio.unal.edu.co/browse?type=author&amp;value=Cubides%20Guerrero,%20Pablo%20Andres</t>
         </is>
@@ -1606,15 +1409,12 @@
       <c r="A66" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B66" t="n">
-        <v>65</v>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Luis Antonio Zuluaga Ramirez</t>
+        </is>
       </c>
       <c r="C66" t="inlineStr">
-        <is>
-          <t>Luis Antonio Zuluaga Ramirez</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
         <is>
           <t>https://scholar.google.com/citations?user=J8t2yvEAAAAJ&amp;hl=es</t>
         </is>
@@ -1624,15 +1424,12 @@
       <c r="A67" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B67" t="n">
-        <v>66</v>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Ivan Rene Delgado Gonzalez</t>
+        </is>
       </c>
       <c r="C67" t="inlineStr">
-        <is>
-          <t>Ivan Rene Delgado Gonzalez</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
         <is>
           <t>https://independent.academia.edu/IvanReneDelgadoGonzalez</t>
         </is>
@@ -1642,15 +1439,12 @@
       <c r="A68" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="B68" t="n">
-        <v>67</v>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Juan David Sierra Arias</t>
+        </is>
       </c>
       <c r="C68" t="inlineStr">
-        <is>
-          <t>Juan David Sierra Arias</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
         <is>
           <t>https://www.tusclases.co/profesores/juan-david-sierra-arias.htm</t>
         </is>
@@ -1660,15 +1454,12 @@
       <c r="A69" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="B69" t="n">
-        <v>68</v>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Cristian Raul Amaya Alba</t>
+        </is>
       </c>
       <c r="C69" t="inlineStr">
-        <is>
-          <t>Cristian Raul Amaya Alba</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
         <is>
           <t>https://estudiantes2016.grupocerros.org/deportista/atleta/75971#/ficha/75971</t>
         </is>
@@ -1678,15 +1469,12 @@
       <c r="A70" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="B70" t="n">
-        <v>69</v>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Cristian Danilo Ramirez Vargas</t>
+        </is>
       </c>
       <c r="C70" t="inlineStr">
-        <is>
-          <t>Cristian Danilo Ramirez Vargas</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
         <is>
           <t>https://repositorio.unal.edu.co/handle/unal/81538</t>
         </is>
@@ -1696,15 +1484,12 @@
       <c r="A71" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="B71" t="n">
-        <v>70</v>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Nestor Orlando Romero Arismendi</t>
+        </is>
       </c>
       <c r="C71" t="inlineStr">
-        <is>
-          <t>Nestor Orlando Romero Arismendi</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
         <is>
           <t>https://www.researchgate.net/profile/Nestor-Arismendi</t>
         </is>
@@ -1714,15 +1499,12 @@
       <c r="A72" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="B72" t="n">
-        <v>71</v>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Daniel Fernando Diaz Romero</t>
+        </is>
       </c>
       <c r="C72" t="inlineStr">
-        <is>
-          <t>Daniel Fernando Diaz Romero</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
         <is>
           <t>https://co.pinterest.com/danielfernandodiazromero/</t>
         </is>
@@ -1732,15 +1514,12 @@
       <c r="A73" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B73" t="n">
-        <v>72</v>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Ivan Felipe Agudelo Amaya</t>
+        </is>
       </c>
       <c r="C73" t="inlineStr">
-        <is>
-          <t>Ivan Felipe Agudelo Amaya</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
         <is>
           <t>https://losestudiantes.com/universidad-nacional/professors/ivan-felipe-agudelo-amaya</t>
         </is>
@@ -1750,15 +1529,12 @@
       <c r="A74" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="B74" t="n">
-        <v>74</v>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Jhonatan Alexis Saldarriaga Conde</t>
+        </is>
       </c>
       <c r="C74" t="inlineStr">
-        <is>
-          <t>Jhonatan Alexis Saldarriaga Conde</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
         <is>
           <t>https://slideplayer.es/slide/5406921/</t>
         </is>
@@ -1768,15 +1544,12 @@
       <c r="A75" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="B75" t="n">
-        <v>75</v>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Carlos Andres Murcia Cañon</t>
+        </is>
       </c>
       <c r="C75" t="inlineStr">
-        <is>
-          <t>Carlos Andres Murcia Cañon</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
         <is>
           <t>https://es-la.facebook.com/carlosandres.murciacanon/</t>
         </is>
@@ -1786,15 +1559,12 @@
       <c r="A76" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B76" t="n">
-        <v>76</v>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Oscar Mauricio Diaz Rincón</t>
+        </is>
       </c>
       <c r="C76" t="inlineStr">
-        <is>
-          <t>Oscar Mauricio Diaz Rincón</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
         <is>
           <t>https://es-la.facebook.com/oscarmauricio.rincondiaz.7/</t>
         </is>
@@ -1804,15 +1574,12 @@
       <c r="A77" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="B77" t="n">
-        <v>77</v>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Diego Fernando Escobar Sarmiento</t>
+        </is>
       </c>
       <c r="C77" t="inlineStr">
-        <is>
-          <t>Diego Fernando Escobar Sarmiento</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
         <is>
           <t>https://www.youtube.com/channel/UCjJBbhPuSFzUdNQwR7bUQGQ</t>
         </is>
@@ -1822,15 +1589,12 @@
       <c r="A78" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B78" t="n">
-        <v>78</v>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Camilo Andres Avila Torres</t>
+        </is>
       </c>
       <c r="C78" t="inlineStr">
-        <is>
-          <t>Camilo Andres Avila Torres</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
         <is>
           <t>https://m.facebook.com/people/Camilo-Andres-Avila-Torres/100080724494896/</t>
         </is>
@@ -1840,15 +1604,12 @@
       <c r="A79" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B79" t="n">
-        <v>79</v>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Ana Maria Garcia Castro</t>
+        </is>
       </c>
       <c r="C79" t="inlineStr">
-        <is>
-          <t>Ana Maria Garcia Castro</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
         <is>
           <t>https://www.funcionpublica.gov.co/web/sigep/hdv/-/directorio/S1500877-4252-4/view</t>
         </is>
@@ -1858,15 +1619,12 @@
       <c r="A80" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B80" t="n">
-        <v>80</v>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Lorena Cortés Páez</t>
+        </is>
       </c>
       <c r="C80" t="inlineStr">
-        <is>
-          <t>Lorena Cortés Páez</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
         <is>
           <t>https://www.facebook.com/lorenacortesp/?locale=es_LA</t>
         </is>
@@ -1876,15 +1634,12 @@
       <c r="A81" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="B81" t="n">
-        <v>81</v>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>David Wilson Romero Guzman</t>
+        </is>
       </c>
       <c r="C81" t="inlineStr">
-        <is>
-          <t>David Wilson Romero Guzman</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
         <is>
           <t>https://research.vu.nl/en/persons/david-wilson-romero-guzman</t>
         </is>
@@ -1894,15 +1649,12 @@
       <c r="A82" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="B82" t="n">
-        <v>82</v>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Fabian Santos Bohorquez</t>
+        </is>
       </c>
       <c r="C82" t="inlineStr">
-        <is>
-          <t>Fabian Santos Bohorquez</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
         <is>
           <t>https://www.facebook.com/fabian.santosbohorquez/</t>
         </is>
@@ -1912,15 +1664,12 @@
       <c r="A83" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="B83" t="n">
-        <v>83</v>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Edwin Fernando Sanabria Marroquin</t>
+        </is>
       </c>
       <c r="C83" t="inlineStr">
-        <is>
-          <t>Edwin Fernando Sanabria Marroquin</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
         <is>
           <t>https://www.larepublica.co/responsabilidad-social/lombricultura-y-un-albergue-las-apuestas-de-odebrecht-por-el-desarrollo-sostenible-2105025</t>
         </is>
@@ -1930,15 +1679,12 @@
       <c r="A84" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="B84" t="n">
-        <v>84</v>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Sergio Andres Rodriguez Rojas</t>
+        </is>
       </c>
       <c r="C84" t="inlineStr">
-        <is>
-          <t>Sergio Andres Rodriguez Rojas</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
         <is>
           <t>https://es-la.facebook.com/public/Sergio-Andres-Rodriguez-Rojas</t>
         </is>
@@ -1948,15 +1694,12 @@
       <c r="A85" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B85" t="n">
-        <v>85</v>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Froilan David Villarreal Barreto</t>
+        </is>
       </c>
       <c r="C85" t="inlineStr">
-        <is>
-          <t>Froilan David Villarreal Barreto</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
         <is>
           <t>https://m.facebook.com/froilan.barreto/</t>
         </is>
@@ -1966,15 +1709,12 @@
       <c r="A86" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="B86" t="n">
-        <v>86</v>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Jessica Fernanda Salguero Ramirez</t>
+        </is>
       </c>
       <c r="C86" t="inlineStr">
-        <is>
-          <t>Jessica Fernanda Salguero Ramirez</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
         <is>
           <t>https://www.facebook.com/jessica.ramirezsalguero.9/?locale=es_LA</t>
         </is>
@@ -1984,15 +1724,12 @@
       <c r="A87" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="B87" t="n">
-        <v>87</v>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>William Alexander Vaquiro Mendoza</t>
+        </is>
       </c>
       <c r="C87" t="inlineStr">
-        <is>
-          <t>William Alexander Vaquiro Mendoza</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
         <is>
           <t>https://www1.upme.gov.co/Entornoinstitucional/Documents/contratistas/Informe_contractual_persona_natural_31Julio2022.pdf</t>
         </is>
@@ -2002,15 +1739,12 @@
       <c r="A88" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B88" t="n">
-        <v>88</v>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Gabriel Fernando Talero Rojas</t>
+        </is>
       </c>
       <c r="C88" t="inlineStr">
-        <is>
-          <t>Gabriel Fernando Talero Rojas</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
         <is>
           <t>https://losestudiantes.com/universidad-nacional/professors/gabriel-fernando-talero-rojas</t>
         </is>
@@ -2020,15 +1754,12 @@
       <c r="A89" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="B89" t="n">
-        <v>89</v>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Freddy Hernan Martinez Quiñones</t>
+        </is>
       </c>
       <c r="C89" t="inlineStr">
-        <is>
-          <t>Freddy Hernan Martinez Quiñones</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
         <is>
           <t>https://www.tecnoempleo.com/freddy-hernan-martinez-quinones.mpt</t>
         </is>
@@ -2038,15 +1769,12 @@
       <c r="A90" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="B90" t="n">
-        <v>90</v>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>David Andres Rivas Tabares</t>
+        </is>
       </c>
       <c r="C90" t="inlineStr">
-        <is>
-          <t>David Andres Rivas Tabares</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
         <is>
           <t>https://scholar.google.com/citations?user=JQ3uv50AAAAJ&amp;hl=en</t>
         </is>
@@ -2056,15 +1784,12 @@
       <c r="A91" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="B91" t="n">
-        <v>91</v>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Laura Hidalgo Hurtado</t>
+        </is>
       </c>
       <c r="C91" t="inlineStr">
-        <is>
-          <t>Laura Hidalgo Hurtado</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
         <is>
           <t>https://www.tiktok.com/@lhh10</t>
         </is>
@@ -2074,15 +1799,12 @@
       <c r="A92" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="B92" t="n">
-        <v>92</v>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Edward Andrey Páez Reyes</t>
+        </is>
       </c>
       <c r="C92" t="inlineStr">
-        <is>
-          <t>Edward Andrey Páez Reyes</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
         <is>
           <t>https://www.facebook.com/BolivianaDeAviacion/photos/a.122628174529/10153028357279530/?type=3</t>
         </is>
@@ -2092,15 +1814,12 @@
       <c r="A93" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="B93" t="n">
-        <v>93</v>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Oscar Alejandro Ochoa Guzman</t>
+        </is>
       </c>
       <c r="C93" t="inlineStr">
-        <is>
-          <t>Oscar Alejandro Ochoa Guzman</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
         <is>
           <t>https://co.pinterest.com/oaochoaguzman/</t>
         </is>
@@ -2110,15 +1829,12 @@
       <c r="A94" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="B94" t="n">
-        <v>94</v>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Robinson Bryan Rubio Parada</t>
+        </is>
       </c>
       <c r="C94" t="inlineStr">
-        <is>
-          <t>Robinson Bryan Rubio Parada</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
         <is>
           <t>https://www.google.com/search?q=Robinson+Bryan+Rubio+Parada&amp;sca_esv=570303733&amp;source=hp&amp;ei=aw4cZevxJJbHkPIP1eCU8Ac&amp;iflsig=AO6bgOgAAAAAZRwce6_H21dx0MvxNJwZuH4DM7vyjvIA&amp;ved=0ahUKEwir06XY9dmBAxWWI0QIHVUwBX4Q4dUDCAo&amp;uact=5&amp;oq=Robinson+Bryan+Rubio+Parada&amp;gs_lp=Egdnd3Mtd2l6IhtSb2JpbnNvbiBCcnlhbiBSdWJpbyBQYXJhZGFIMlAAWCNwAHgAkAEAmAEAoAEAqgEAuAEDyAEA-AEB&amp;sclient=gws-wiz</t>
         </is>
@@ -2128,15 +1844,12 @@
       <c r="A95" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="B95" t="n">
-        <v>95</v>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Andres Alfonso Barrios Bernal</t>
+        </is>
       </c>
       <c r="C95" t="inlineStr">
-        <is>
-          <t>Andres Alfonso Barrios Bernal</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
         <is>
           <t>https://www.instagram.com/andresbarriosbernal/?hl=es-la</t>
         </is>
@@ -2146,15 +1859,12 @@
       <c r="A96" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="B96" t="n">
-        <v>96</v>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Cesar Augusto Niño Molina</t>
+        </is>
       </c>
       <c r="C96" t="inlineStr">
-        <is>
-          <t>Cesar Augusto Niño Molina</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
         <is>
           <t>http://www.datajuridica.com/CESAR_AUGUSTO_NI%C3%91O.htm</t>
         </is>
@@ -2164,15 +1874,12 @@
       <c r="A97" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="B97" t="n">
-        <v>97</v>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Jose Andres Jaimes Sarmiento</t>
+        </is>
       </c>
       <c r="C97" t="inlineStr">
-        <is>
-          <t>Jose Andres Jaimes Sarmiento</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
         <is>
           <t>https://co.pinterest.com/jajaimess/</t>
         </is>
@@ -2182,15 +1889,12 @@
       <c r="A98" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="B98" t="n">
-        <v>98</v>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Sebastian Eduardo Chaparro Cuevas</t>
+        </is>
       </c>
       <c r="C98" t="inlineStr">
-        <is>
-          <t>Sebastian Eduardo Chaparro Cuevas</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
         <is>
           <t>https://repositorio.unal.edu.co/handle/unal/79872</t>
         </is>
@@ -2200,15 +1904,12 @@
       <c r="A99" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="B99" t="n">
-        <v>99</v>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Leonel Armando Vinasco Zapata</t>
+        </is>
       </c>
       <c r="C99" t="inlineStr">
-        <is>
-          <t>Leonel Armando Vinasco Zapata</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
         <is>
           <t>https://www.researchgate.net/profile/Leonel-Armando-Vinasco-Zapata</t>
         </is>
@@ -2216,17 +1917,14 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="B100" t="n">
-        <v>200</v>
+        <v>100</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Julian Enrique Nieto Rodriguez</t>
+        </is>
       </c>
       <c r="C100" t="inlineStr">
-        <is>
-          <t>Julian Enrique Nieto Rodriguez</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
         <is>
           <t>https://profiles.jobomas.com/julian.enrique.nieto.rodriguez</t>
         </is>
@@ -2234,17 +1932,14 @@
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="B101" t="n">
-        <v>201</v>
+        <v>101</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Leonardo Andres Rodriguez Forero</t>
+        </is>
       </c>
       <c r="C101" t="inlineStr">
-        <is>
-          <t>Leonardo Andres Rodriguez Forero</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
         <is>
           <t>https://www.facebook.com/leonardorodfor/?locale=es_LA</t>
         </is>
@@ -2252,17 +1947,14 @@
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>202</v>
-      </c>
-      <c r="B102" t="n">
-        <v>202</v>
+        <v>102</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Mauricio Andres Molina Moreno</t>
+        </is>
       </c>
       <c r="C102" t="inlineStr">
-        <is>
-          <t>Mauricio Andres Molina Moreno</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
         <is>
           <t>https://www.slideshare.net/maomolina14</t>
         </is>
@@ -2270,17 +1962,14 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>203</v>
-      </c>
-      <c r="B103" t="n">
-        <v>203</v>
+        <v>103</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Yenny Disney Moyano Lopez</t>
+        </is>
       </c>
       <c r="C103" t="inlineStr">
-        <is>
-          <t>Yenny Disney Moyano Lopez</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
         <is>
           <t>https://profiles.jobomas.com/yenny.disney.moyano.lopez.moyano.lopez</t>
         </is>
@@ -2288,17 +1977,14 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>204</v>
-      </c>
-      <c r="B104" t="n">
-        <v>204</v>
+        <v>104</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Ceudiel Alexis Valero Portilla</t>
+        </is>
       </c>
       <c r="C104" t="inlineStr">
-        <is>
-          <t>Ceudiel Alexis Valero Portilla</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
         <is>
           <t>https://repositorio.unbosque.edu.co/handle/20.500.12495/6586</t>
         </is>
@@ -2306,17 +1992,14 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>205</v>
-      </c>
-      <c r="B105" t="n">
-        <v>205</v>
+        <v>105</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Andrés Eduardo Tuta López</t>
+        </is>
       </c>
       <c r="C105" t="inlineStr">
-        <is>
-          <t>Andrés Eduardo Tuta López</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
         <is>
           <t>https://slideplayer.es/slide/5545782/</t>
         </is>
@@ -2324,17 +2007,14 @@
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>206</v>
-      </c>
-      <c r="B106" t="n">
-        <v>206</v>
+        <v>106</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Fabian Leonardo Aguilar Aguilar</t>
+        </is>
       </c>
       <c r="C106" t="inlineStr">
-        <is>
-          <t>Fabian Leonardo Aguilar Aguilar</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
         <is>
           <t>https://repositorio.uniandes.edu.co/handle/1992/52332/browse?authority=c5ce1008-1f53-493a-88db-6ac081585b72&amp;type=author</t>
         </is>
@@ -2342,17 +2022,14 @@
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>207</v>
-      </c>
-      <c r="B107" t="n">
-        <v>207</v>
+        <v>107</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Daniel Fernandez Vera</t>
+        </is>
       </c>
       <c r="C107" t="inlineStr">
-        <is>
-          <t>Daniel Fernandez Vera</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
         <is>
           <t>https://www.facebook.com/daniel.fernandezvera.739/?locale=es_LA</t>
         </is>
@@ -2360,17 +2037,14 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>208</v>
-      </c>
-      <c r="B108" t="n">
-        <v>208</v>
+        <v>108</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Kevin Stid Ramirez Garzón</t>
+        </is>
       </c>
       <c r="C108" t="inlineStr">
-        <is>
-          <t>Kevin Stid Ramirez Garzón</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
         <is>
           <t>https://prezi.com/p/faycwqydshnd/entropia/</t>
         </is>
@@ -2378,17 +2052,14 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>209</v>
-      </c>
-      <c r="B109" t="n">
-        <v>209</v>
+        <v>109</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Jorge Luis Doria Ortiz</t>
+        </is>
       </c>
       <c r="C109" t="inlineStr">
-        <is>
-          <t>Jorge Luis Doria Ortiz</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
         <is>
           <t>https://m.facebook.com/people/Jorge-Luis-Doria-Ortiz/804618878/</t>
         </is>
@@ -2396,17 +2067,14 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>210</v>
-      </c>
-      <c r="B110" t="n">
-        <v>210</v>
+        <v>110</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>Andrea Suaza Montalvo</t>
+        </is>
       </c>
       <c r="C110" t="inlineStr">
-        <is>
-          <t>Andrea Suaza Montalvo</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
         <is>
           <t>https://scholar.google.com/citations?user=d3eKzx4AAAAJ&amp;hl=es</t>
         </is>
@@ -2414,17 +2082,14 @@
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>211</v>
-      </c>
-      <c r="B111" t="n">
-        <v>211</v>
+        <v>111</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Nicolas Cuervo Benavides</t>
+        </is>
       </c>
       <c r="C111" t="inlineStr">
-        <is>
-          <t>Nicolas Cuervo Benavides</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
         <is>
           <t>https://www.instagram.com/primer_cuervo/</t>
         </is>
@@ -2432,17 +2097,14 @@
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>212</v>
-      </c>
-      <c r="B112" t="n">
-        <v>212</v>
+        <v>112</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>David Esteban Figueredo Ramirez</t>
+        </is>
       </c>
       <c r="C112" t="inlineStr">
-        <is>
-          <t>David Esteban Figueredo Ramirez</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
         <is>
           <t>https://www.youtube.com/channel/UCGx38XifjT-U0IRvz5fZvNA</t>
         </is>
@@ -2450,17 +2112,14 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>213</v>
-      </c>
-      <c r="B113" t="n">
-        <v>213</v>
+        <v>113</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Luis Ernesto Sanchez Amaya</t>
+        </is>
       </c>
       <c r="C113" t="inlineStr">
-        <is>
-          <t>Luis Ernesto Sanchez Amaya</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
         <is>
           <t>https://www.google.com/search?q=Luis+Ernesto+Sanchez+Amaya&amp;sca_esv=570303733&amp;source=hp&amp;ei=2BAcZfTwKPnGkPIPm-KT6A0&amp;iflsig=AO6bgOgAAAAAZRwe6OT8DSZr3Qzc6vvyGWqhLk8L1Ehb&amp;ved=0ahUKEwj0vLiA-NmBAxV5I0QIHRvxBN0Q4dUDCAo&amp;uact=5&amp;oq=Luis+Ernesto+Sanchez+Amaya&amp;gs_lp=Egdnd3Mtd2l6IhpMdWlzIEVybmVzdG8gU2FuY2hleiBBbWF5YUg4UABYJnAAeACQAQCYAQCgAQCqAQC4AQPIAQD4AQE&amp;sclient=gws-wiz</t>
         </is>
@@ -2468,17 +2127,14 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>214</v>
-      </c>
-      <c r="B114" t="n">
-        <v>214</v>
+        <v>114</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Ivan Oswaldo Penagos Jimenez</t>
+        </is>
       </c>
       <c r="C114" t="inlineStr">
-        <is>
-          <t>Ivan Oswaldo Penagos Jimenez</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
         <is>
           <t>https://catalogo.uexternado.edu.co/cgi-bin/koha/opac-detail.pl?biblionumber=77610&amp;shelfbrowse_itemnumber=101707</t>
         </is>
@@ -2486,17 +2142,14 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>215</v>
-      </c>
-      <c r="B115" t="n">
-        <v>215</v>
+        <v>115</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Carlos Andres Pinzon Loaiza</t>
+        </is>
       </c>
       <c r="C115" t="inlineStr">
-        <is>
-          <t>Carlos Andres Pinzon Loaiza</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
         <is>
           <t>https://erasmusu.com/it/carlos-andres-pinzon-loaiza-1300205</t>
         </is>
@@ -2504,17 +2157,14 @@
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>221</v>
-      </c>
-      <c r="B116" t="n">
-        <v>221</v>
+        <v>121</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Eliana Marcela Gómez Navarrete</t>
+        </is>
       </c>
       <c r="C116" t="inlineStr">
-        <is>
-          <t>Eliana Marcela Gómez Navarrete</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
         <is>
           <t>https://losestudiantes.com/universidad-nacional/professors/eliana-marcela-gomez-navarrete</t>
         </is>
@@ -2522,17 +2172,14 @@
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>227</v>
-      </c>
-      <c r="B117" t="n">
-        <v>227</v>
+        <v>127</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Monica Estefania Girardot Camargo</t>
+        </is>
       </c>
       <c r="C117" t="inlineStr">
-        <is>
-          <t>Monica Estefania Girardot Camargo</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
         <is>
           <t>https://www.virtualpro.co/noticias/fabrican-aleacion-de-niquel-valiosa-para-la-industria</t>
         </is>
@@ -2540,17 +2187,14 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>229</v>
-      </c>
-      <c r="B118" t="n">
-        <v>229</v>
+        <v>129</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Fabian Eduardo Ramos Torres</t>
+        </is>
       </c>
       <c r="C118" t="inlineStr">
-        <is>
-          <t>Fabian Eduardo Ramos Torres</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
         <is>
           <t>https://www.uac.edu.co/pregrado/ingenieria-industrial/</t>
         </is>
@@ -2558,17 +2202,14 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>232</v>
-      </c>
-      <c r="B119" t="n">
-        <v>232</v>
+        <v>132</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Darling Katherine Rubio Ortiz</t>
+        </is>
       </c>
       <c r="C119" t="inlineStr">
-        <is>
-          <t>Darling Katherine Rubio Ortiz</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
         <is>
           <t>https://www.sciencedirect.com/science/article/abs/pii/S0308814620302417</t>
         </is>
@@ -2576,17 +2217,14 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>236</v>
-      </c>
-      <c r="B120" t="n">
-        <v>236</v>
+        <v>136</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Luis Ernesto Sanchez Amaya</t>
+        </is>
       </c>
       <c r="C120" t="inlineStr">
-        <is>
-          <t>Luis Ernesto Sanchez Amaya</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
         <is>
           <t>https://www.google.com/search?q=Luis+Ernesto+Sanchez+Amaya&amp;sca_esv=570352775&amp;source=hp&amp;ei=ShgcZayjMrrikPIPpbGA8A4&amp;iflsig=AO6bgOgAAAAAZRwmWs2zAy2lVf4TNyXHyPlVgSdOmSF7&amp;ved=0ahUKEwis8K6N_9mBAxU6MUQIHaUYAO4Q4dUDCAo&amp;uact=5&amp;oq=Luis+Ernesto+Sanchez+Amaya&amp;gs_lp=Egdnd3Mtd2l6IhpMdWlzIEVybmVzdG8gU2FuY2hleiBBbWF5YUg1UABYJ3AAeACQAQCYAQCgAQCqAQC4AQPIAQD4AQE&amp;sclient=gws-wiz&amp;bshm=rimc/1</t>
         </is>
@@ -2594,17 +2232,14 @@
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>237</v>
-      </c>
-      <c r="B121" t="n">
-        <v>237</v>
+        <v>137</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Rodrigo Achury Duarte</t>
+        </is>
       </c>
       <c r="C121" t="inlineStr">
-        <is>
-          <t>Rodrigo Achury Duarte</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr">
         <is>
           <t>https://www.youtube.com/channel/UC3bow_RbXEBVriUFhIU22nw</t>
         </is>
@@ -2612,19 +2247,1201 @@
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>240</v>
-      </c>
-      <c r="B122" t="n">
-        <v>240</v>
+        <v>140</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Heiver Andres Torres Rincon</t>
+        </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Heiver Andres Torres Rincon</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
           <t>https://construyored.com/profesionales/42599-heiver-andres-torres-rincon</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Carlos Javier Enriquez Chenas</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/carlos.ec.50/?locale=es_LA</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Julián David Hernández Tovar</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/julian.d.hernandez.12/?locale=en_GB</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Javier Enrique Ibáñez Ortiz</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>https://m.facebook.com/public/Javier-Enrique-Ib%C3%A1%C3%B1ez-Ortiz?locale2=es_LA</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Mauro Herrera Pupo</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/maurohe26/</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Andres Felipe Serrano Medina</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>https://repositorio.unal.edu.co/handle/unal/83425</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Vladimir Cárdenas Bocanegra</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>https://repositorio.unal.edu.co/browse?type=author&amp;value=C%C3%A1rdenas%20Bocanegra,%20Vladimir%20Alfonso</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Johan José Castañeda Vega</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>https://es-la.facebook.com/public/Jose-Johan-Casta%C3%B1eda</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Favian Henrike Angarita Cubillos</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>http://bienestar.bogota.unal.edu.co/pdf/gestion/d83_0905170400_adj_ged.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Jesus Emilio Mojica Galvis</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>https://www.academia.edu/4726764/DETERIORO_DE_ECOSISTEMAS_Y_P%C3%89RDIDA_DE_BIODIVERSIDAD_articulo_final</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Juan Fernando Bohórquez Rodríguez</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>https://co.pinterest.com/jbohrquezrodrguez/</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>151</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Alvaro Raul Montaña Olivares</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>https://repositorio.escuelaing.edu.co/handle/001/765/statistics?locale-attribute=es</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Hector Camilo Higuera Florez</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>https://www.ucatolica.edu.co/portal/Docente/hector-camilo-higuera-florez/</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Maria Paula Sierra Caceres</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>https://es-es.facebook.com/public/Maria-Paula-Sierra-Caceres</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>154</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Nelson Alejandro Rincon Pinzon</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>https://unal.academia.edu/NelsonAlejandroRinconPinzon</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Maribel Rocio Romero De La Hoz</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>https://independent.academia.edu/MaribelRocioRomeroDeLaHoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>156</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>David Esteban Garzon Rincon</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>https://co.pinterest.com/davidestebangarzonrincon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Giovanny Fermin Albarracín Riveros</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>https://torre.ai/albarracingiovanny?r=IqqthgZe</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Miguel Ángel Rivas Tabares</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>https://repositorio.unal.edu.co/browse?type=author&amp;value=Rivas%20Tabares,%20Miguel%20%C3%81ngel</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>159</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Ricardo Alfonso Villamizar Saenz</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>https://profiles.jobomas.com/ricardo.alfonso.villamizar.saenz</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Fabian Ricardo Sierra Gonzalez</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>https://m.facebook.com/fabian.r.gonzalez.52/</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Sergio Steven Lopez Martinez</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>https://dblp.org/pid/226/7588.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>162</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Eurlin Alejandro Avila Becerra</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>https://construyored.com/profesionales/23549-eurlin-alejandro-avila-becerra</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>163</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Joseph Steven Zambrano Contreras</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>https://repositorio.uniandes.edu.co/browse?authority=f4d5c903-8a02-4fbe-a319-09882b0ae5a6&amp;type=author</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Carlos Leonardo Sarmiento Alcala</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>https://peaku.co/es/cv/68236-carlos-leonardo-sarmiento-alcala</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Juan Esteban Ramirez Gonzalez</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>https://www.researchgate.net/profile/Juan-Esteban-Ramirez-Gonzalez</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Saúl Gregory Mendieta Galindo</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/saulgregory.mendietagalindo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>167</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Fabian Andres Rodriguez Becerra</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>https://www.worldcubeassociation.org/persons/2012BECE01</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>168</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Diego Alejandro Sanchez Rodriguez</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>https://www.transfermarkt.co/diego-sanchez/profil/spieler/570524</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>169</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>William Alfonso Suarez Ortiz</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>https://losestudiantes.com/universidad-nacional/professors/william-alfonso-suarez-ortiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Jhovany Andres Amaya Peña</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>https://research-hub.urosario.edu.co/display/n79627258</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Daniel Steeven Muñoz Castro</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>https://www.researchgate.net/profile/Daniel-Munoz-Castro</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Ivan Dario Torres Rodriguez</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>https://m.facebook.com/ivandario.torresrodriguez/</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Héctor Augusto Daza Roa</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>https://www.elespectador.com/judicial/desarticulan-banda-que-enviaba-cocaina-a-eeuu-y-a-europa-article-461963/</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Juan Felipe Loaiza Cardona</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>https://m.facebook.com/juanfelipe.cardonaloaiza.7/</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Nicholas Fernando Aristizabal Mejia</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>https://www.bogotaabierta.gov.co/313-nicholas-fernando-aristizabal-mejia/perfil</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Julio Cesar Cortes Sanchez</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>https://es-la.facebook.com/juliocesar.cortessanchez/</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Jonathan Alexander Gomez Rodriguez</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>https://www.tusclases.co/profesores/jonathan-alexander-gomez.htm</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Alexander Chaparro Romero</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>https://siesia.unal.edu.co/alumni/m/resume/view/curriculum_alexander_chaparro_romero</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Juan Felipe Valdión Epia</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=Juan+Felipe+Valdi%C3%B3n+Epia&amp;sca_esv=570352775&amp;source=hp&amp;ei=LB8cZZqVMbvF0PEP6_6-iA4&amp;iflsig=AO6bgOgAAAAAZRwtPLt2IYNeHQfWWWD1z0RxzT4EBYtt&amp;ved=0ahUKEwia28XVhdqBAxW7IjQIHWu_D-EQ4dUDCAo&amp;uact=5&amp;oq=Juan+Felipe+Valdi%C3%B3n+Epia&amp;gs_lp=Egdnd3Mtd2l6IhlKdWFuIEZlbGlwZSBWYWxkacOzbiBFcGlhSDRQAFgkcAB4AJABAJgBAKABAKoBALgBA8gBAPgBAQ&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>360</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Juan Fernando Lopez Prieto</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/juanfernando.prietolopez.9/?locale=es_ES</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>361</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Hollman Andres Rodriguez Torres</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/user/andres130995/channels?app=desktop&amp;view=56&amp;shelf_id=0</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>362</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>William Esteban Figueroa Beltran</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>https://prezi.com/00ad04zyuuwk/mi-contexto-de-formacion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>363</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Ivan Dario Sanchez Cifuentes</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/ivandariosanchezcifuentes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>364</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Jenny Andrea Diaz Ramirez</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/jenny.a.ramirez.5/?locale=es_LA</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>365</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Monica Alejandra Castillo Sanchez</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>https://co.pinterest.com/macastillocertecnica/</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>366</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Manuel Camilo Chala Penagos</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>https://riubu.ubu.es/handle/10259.4/104/browse?authority=f975fe02-8076-4251-9ec8-3f883ca3bb72&amp;type=author&amp;locale-attribute=fr</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>367</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Juan Sebastián Delgado Caicedo</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/juansebastian.delgadocaicedo/?locale=hi_IN</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>368</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Cristian Camilo Peñaloza Cespedes</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>https://www.fiscalia.gov.co/colombia/wp-content/uploads/2014/12/2014-05-19-SENTENCIA-BLOQUE-TOLIMA-07-05-14-PERJ..pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>369</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Gabriel Jaime Becerra Eslava</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/gjbecerrae/</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>370</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Diego Fernando Romero Obando</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>https://repository.eafit.edu.co/handle/10784/31900</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>371</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Jhonatan Andrés Alvear Estrada</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>https://twitter.com/i/flow/login?redirect_after_login=%2Falvearestrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>372</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Jesus Nicolas Moreno Franco</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>https://unal.academia.edu/JesusNicolasMorenoFranco</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>373</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Carlos Esteban Hernandez Cordoba</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>https://estudiantes2012.grupocerros.org/deportista/atleta/42246#/ficha/42246</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>374</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Lizzy Tengana Hurtado</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>https://scholar.google.com/citations?user=khrWyz0AAAAJ&amp;hl=en</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>375</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Francisco Julian Sandoval Avila</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>https://repositorio.unal.edu.co/handle/unal/75449/browse?type=author&amp;value=Sandoval+%C3%81vila%2C+Francisco+Juli%C3%A1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>376</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Pablo Daniel Charry Barrero</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>https://m.facebook.com/SenalCalafate/photos/fortalecer-culturanacion-lanz%C3%B3-un-programa-de-apoyo-para-artistas-y-trabajadores/644739969467949/?locale=nl_NL</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>377</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Camila Alejandra Jimenez Bejarano</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>https://www.tusclases.co/profesores/camila-jimenez-jimenez-bejarano.htm</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>378</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Nestor Isaac Maldonado Mora</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>https://inm.gov.co/web/wp-content/uploads/2022/01/RESOL.-023-DE-NOMBRAMIENTO-NESTOR-MALDONADO.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>1228</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Oscar Andrés Espinosa Serrano</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>https://inshaka.com/miperfil/Oscar</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>1229</v>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Camilo Andres Prieto Peña</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>https://rocketreach.co/camilo-andres-prieto-pena-email_362229304</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>1230</v>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Carlos Eduardo Mosquera Noguera</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/carloseduardo.mosqueranoguera/</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>1231</v>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Juan Carlos Quitian Romero</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>https://www.uniboyaca.edu.co/es/facultad-de-ciencias-e-ingenieria</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>1232</v>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Kory Stephany Castro Muñoz</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>https://www.igac.gov.co/es/contenido/resolucion-598-de-2020-kory-stephany-castro-munoz</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>1233</v>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Álvaro Javier Gallardo Guerrero</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>https://revistas.sena.edu.co/index.php/conciencia/search/authors/view?givenName=Alvaro%20Javier%20&amp;familyName%5B%5D=Gallardo%20Guerrero&amp;affiliation=Facilitador%20&amp;country=CO&amp;authorName=Gallardo%20Guerrero%2C%20Alvaro%20Javier%20</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Camilo Andres Lozano Prada</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/camilo.l.prada/?locale=es_LA</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>1235</v>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>German Joaquin Bernal Escalante</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>https://gw.geneanet.org/epareja?lang=en&amp;n=bernal+escalante&amp;oc=0&amp;p=tomas+jose+joaquin</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>1236</v>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Miguel Angel Perez Sarmiento</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>https://es.wikipedia.org/wiki/Miguel_%C3%81ngel_P%C3%A9rez_Sarmiento</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>1237</v>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Ricardo Amezquita Reyes</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>https://torre.ai/amezquitaricardo3?r=d3uDEvRe</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>1238</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Daniel Arturo Diaz Sarmiento</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>https://www.academia.edu/5850966/Datos_Laboratorio_Agregados</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>1239</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Sergio Andres Quecan Diaz</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>https://grupoestudiounal.webnode.com.co/products/sergio-andres-quecan-diaz-/</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Andres Felipe Borrero Gutierrez</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/andres.borrerogutierrez/?locale=es_ES</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>1241</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Nathalia Kateryne Tinjaca Jimenez</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>https://repositorio.unal.edu.co/browse?type=author&amp;value=Tinjac%C3%A1%20Jim%C3%A9nez,%20Nathalia%20Kateryne</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>1242</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Jerson Jair Cuevas Bocanegra</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>https://co.pinterest.com/cuevasbocanegra/</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>1243</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Juan Pablo Loaiza Ramírez</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>https://scholar.google.com.co/citations?user=qrUgnPwAAAAJ&amp;hl=es</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>1244</v>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Leonardo Fajardo Osorio</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>https://slideplayer.es/slide/4193722/</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>1245</v>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Nathaly Fernanda Garzon Agudelo</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/NathalyGarzonAgudelo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>1246</v>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Andres Botia Carreño</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>https://www.quora.com/profile/Andr%C3%A9s-Bot%C3%ADa-Carre%C3%B1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>1247</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Daniel Eduardo Roncancio Rubiano</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?q=Daniel+Eduardo+Roncancio+Rubiano&amp;sca_esv=570352775&amp;source=hp&amp;ei=GyQcZb3tOZTW5OUPkbOoiA0&amp;iflsig=AO6bgOgAAAAAZRwyLKGhCGau0ZrqZU1AKyGuU-TolrqH&amp;ved=0ahUKEwj95u2vitqBAxUUK7kGHZEZCtEQ4dUDCAo&amp;uact=5&amp;oq=Daniel+Eduardo+Roncancio+Rubiano&amp;gs_lp=Egdnd3Mtd2l6IiBEYW5pZWwgRWR1YXJkbyBSb25jYW5jaW8gUnViaWFub0hAUABYMHAAeACQAQCYAQCgAQCqAQC4AQPIAQD4AQE&amp;sclient=gws-wiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>1248</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Juan Camilo Neiva Aranguren</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>https://yugiohblog.konami.com/2023/06/south-america-wcq-pairings-for-round-8-4/</t>
         </is>
       </c>
     </row>

</xml_diff>